<commit_message>
corrected three data entries
</commit_message>
<xml_diff>
--- a/data/CSIRO quarantine project data.xlsx
+++ b/data/CSIRO quarantine project data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25714"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1456" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BDD04D7-2FDA-429D-A36C-386B3092F230}"/>
+  <xr:revisionPtr revIDLastSave="1463" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7163DA83-B010-41C5-BA53-E55C6C0D53E7}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master measure sheet" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8364" uniqueCount="2136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8374" uniqueCount="2136">
   <si>
     <t>ID</t>
   </si>
@@ -4316,52 +4315,52 @@
     <t>08_M_02</t>
   </si>
   <si>
+    <t>08_M_03</t>
+  </si>
+  <si>
     <t>C4_1</t>
   </si>
   <si>
-    <t>08_M_03</t>
+    <t>08_M_04</t>
   </si>
   <si>
     <t>C4_2</t>
   </si>
   <si>
-    <t>08_M_04</t>
+    <t>08_M_05</t>
   </si>
   <si>
     <t>C4_3</t>
   </si>
   <si>
-    <t>08_M_05</t>
+    <t>08_M_06</t>
   </si>
   <si>
     <t>C4_4</t>
   </si>
   <si>
-    <t>08_M_06</t>
+    <t>08_M_07</t>
   </si>
   <si>
     <t>C4_5</t>
   </si>
   <si>
-    <t>08_M_07</t>
+    <t>08_M_08</t>
   </si>
   <si>
     <t>C4_6</t>
   </si>
   <si>
-    <t>08_M_08</t>
+    <t>08_M_09</t>
   </si>
   <si>
     <t>C4_7</t>
   </si>
   <si>
-    <t>08_M_09</t>
+    <t>08_M_10</t>
   </si>
   <si>
     <t>C4_8</t>
-  </si>
-  <si>
-    <t>08_M_10</t>
   </si>
   <si>
     <t>C4_9</t>
@@ -8206,13 +8205,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9776,8 +9775,8 @@
   <dimension ref="A1:O1355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A570" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F645" sqref="F645"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1023" sqref="C1023"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39531,6 +39530,12 @@
       <c r="I782" s="1">
         <v>4.29</v>
       </c>
+      <c r="J782" s="9">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K782" s="9" t="s">
+        <v>1425</v>
+      </c>
       <c r="L782" s="24" t="s">
         <v>1426</v>
       </c>
@@ -39569,8 +39574,14 @@
       <c r="I783" s="1">
         <v>3.76</v>
       </c>
+      <c r="J783" s="9">
+        <v>1.2349999999999999</v>
+      </c>
+      <c r="K783" s="9" t="s">
+        <v>1428</v>
+      </c>
       <c r="L783" s="24" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="M783" s="1" t="s">
         <v>747</v>
@@ -39579,7 +39590,7 @@
     </row>
     <row r="784" spans="1:15">
       <c r="A784" s="1" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B784" s="1" t="s">
         <v>20</v>
@@ -39605,8 +39616,14 @@
       <c r="I784" s="1">
         <v>3.2</v>
       </c>
+      <c r="J784" s="9">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="K784" s="9" t="s">
+        <v>1430</v>
+      </c>
       <c r="L784" s="24" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="M784" s="1" t="s">
         <v>747</v>
@@ -39615,7 +39632,7 @@
     </row>
     <row r="785" spans="1:15">
       <c r="A785" s="1" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B785" s="1" t="s">
         <v>20</v>
@@ -39641,8 +39658,14 @@
       <c r="I785" s="1">
         <v>3.78</v>
       </c>
+      <c r="J785" s="9">
+        <v>1.57</v>
+      </c>
+      <c r="K785" s="9" t="s">
+        <v>1432</v>
+      </c>
       <c r="L785" s="24" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="M785" s="1" t="s">
         <v>747</v>
@@ -39651,7 +39674,7 @@
     </row>
     <row r="786" spans="1:15">
       <c r="A786" s="1" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B786" s="1" t="s">
         <v>20</v>
@@ -39677,8 +39700,14 @@
       <c r="I786" s="1">
         <v>3.36</v>
       </c>
+      <c r="J786" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="K786" s="9" t="s">
+        <v>1434</v>
+      </c>
       <c r="L786" s="24" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="M786" s="1" t="s">
         <v>747</v>
@@ -39687,7 +39716,7 @@
     </row>
     <row r="787" spans="1:15">
       <c r="A787" s="1" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="B787" s="1" t="s">
         <v>20</v>
@@ -39713,8 +39742,14 @@
       <c r="I787" s="1">
         <v>3.39</v>
       </c>
+      <c r="J787" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="K787" s="9" t="s">
+        <v>1436</v>
+      </c>
       <c r="L787" s="24" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="M787" s="1" t="s">
         <v>747</v>
@@ -39725,7 +39760,7 @@
     </row>
     <row r="788" spans="1:15">
       <c r="A788" s="1" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B788" s="1" t="s">
         <v>20</v>
@@ -39751,8 +39786,14 @@
       <c r="I788" s="1">
         <v>3.5</v>
       </c>
+      <c r="J788" s="9">
+        <v>0.71500000000000008</v>
+      </c>
+      <c r="K788" s="9" t="s">
+        <v>1438</v>
+      </c>
       <c r="L788" s="24" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="M788" s="1" t="s">
         <v>747</v>
@@ -39761,7 +39802,7 @@
     </row>
     <row r="789" spans="1:15">
       <c r="A789" s="1" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B789" s="1" t="s">
         <v>20</v>
@@ -39787,8 +39828,14 @@
       <c r="I789" s="1">
         <v>3.68</v>
       </c>
+      <c r="J789" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="K789" s="9" t="s">
+        <v>1440</v>
+      </c>
       <c r="L789" s="24" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="M789" s="1" t="s">
         <v>747</v>
@@ -39797,7 +39844,7 @@
     </row>
     <row r="790" spans="1:15">
       <c r="A790" s="1" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B790" s="1" t="s">
         <v>20</v>
@@ -39823,8 +39870,14 @@
       <c r="I790" s="1">
         <v>3.35</v>
       </c>
+      <c r="J790" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="K790" s="9" t="s">
+        <v>1442</v>
+      </c>
       <c r="L790" s="24" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="M790" s="1" t="s">
         <v>747</v>
@@ -39833,7 +39886,7 @@
     </row>
     <row r="791" spans="1:15">
       <c r="A791" s="1" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B791" s="1" t="s">
         <v>20</v>
@@ -39896,6 +39949,12 @@
       </c>
       <c r="I792" s="1">
         <v>3.88</v>
+      </c>
+      <c r="J792" s="9">
+        <v>0.89</v>
+      </c>
+      <c r="K792" s="9" t="s">
+        <v>1445</v>
       </c>
       <c r="L792" s="24" t="s">
         <v>1446</v>

</xml_diff>